<commit_message>
Despues de la reunion 10-3-22
</commit_message>
<xml_diff>
--- a/data/pruebas.xlsx
+++ b/data/pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jlopez\Desktop\facultad\5º\TFG_INF\TFG_PSO\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF3690A-D2A7-4BE5-9187-E954800BE5EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C06E026-2BCB-43B6-8647-EBC4BE8C7973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{08983E8D-A012-4C5C-9888-5099C9EB74F9}"/>
   </bookViews>
@@ -2910,11 +2910,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E5205A3-375B-4BB7-AA25-87972EA27D1E}">
-  <dimension ref="A1:I171"/>
+  <dimension ref="A1:I172"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
+      <pane ySplit="1" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I173" sqref="I173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7167,6 +7167,16 @@
         <v>1.0515666666666668</v>
       </c>
       <c r="I171" s="38"/>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F172">
+        <f xml:space="preserve"> SUM(F2:F171)</f>
+        <v>11518654.200000001</v>
+      </c>
+      <c r="I172">
+        <f>F172/(1000*60)</f>
+        <v>191.97757000000001</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="136">
@@ -7318,8 +7328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7CD5CF8-E0D3-4596-B6F2-746E33A17FA4}">
   <dimension ref="A1:P171"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Para pruebas de tiempos
</commit_message>
<xml_diff>
--- a/data/pruebas.xlsx
+++ b/data/pruebas.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jlopez\Desktop\facultad\5º\TFG_INF\TFG_PSO\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C06E026-2BCB-43B6-8647-EBC4BE8C7973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA29262E-CF07-4710-A119-BA4BF443585A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{08983E8D-A012-4C5C-9888-5099C9EB74F9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="6" xr2:uid="{08983E8D-A012-4C5C-9888-5099C9EB74F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Mediciones Previas" sheetId="1" r:id="rId1"/>
     <sheet name="Mediciones Optimización" sheetId="2" r:id="rId2"/>
-    <sheet name="Tablas" sheetId="3" r:id="rId3"/>
+    <sheet name="Tablas Mediciones" sheetId="3" r:id="rId3"/>
+    <sheet name="Mediciones optimización 2" sheetId="4" r:id="rId4"/>
+    <sheet name="Tablas Mediciones 2" sheetId="5" r:id="rId5"/>
+    <sheet name="Barrido Iteraciones" sheetId="6" r:id="rId6"/>
+    <sheet name="Tablas Barrido Iteraciones" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="35">
   <si>
     <t>N_Partículas</t>
   </si>
@@ -116,6 +120,36 @@
   </si>
   <si>
     <t>Paralelo Con O2 Con SIMD</t>
+  </si>
+  <si>
+    <t>Iteración</t>
+  </si>
+  <si>
+    <t>Mejor K</t>
+  </si>
+  <si>
+    <t>Tasa de Clasificación Media
+15 P</t>
+  </si>
+  <si>
+    <t>Tasa de Clasificación Media
+30 P</t>
+  </si>
+  <si>
+    <t>Tasa de Clasificación Media
+45 P</t>
+  </si>
+  <si>
+    <t>Tasa de Clasificación Media
+60 P</t>
+  </si>
+  <si>
+    <t>Tasa de Clasificación Media
+75 P</t>
+  </si>
+  <si>
+    <t>Tasa de Clasificación Media
+90 P</t>
   </si>
 </sst>
 </file>
@@ -289,7 +323,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -378,13 +412,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -392,6 +426,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -440,7 +480,9 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="tx1"/>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -451,7 +493,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Tablas!$I$3:$P$3</c:f>
+              <c:f>'Tablas Mediciones'!$I$3:$P$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -498,7 +540,9 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -509,7 +553,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Tablas!$I$4:$P$4</c:f>
+              <c:f>'Tablas Mediciones'!$I$4:$P$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -556,7 +600,9 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -567,7 +613,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Tablas!$I$5:$P$5</c:f>
+              <c:f>'Tablas Mediciones'!$I$5:$P$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -625,7 +671,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Tablas!$I$6:$P$6</c:f>
+              <c:f>'Tablas Mediciones'!$I$6:$P$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -683,7 +729,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Tablas!$I$7:$P$7</c:f>
+              <c:f>'Tablas Mediciones'!$I$7:$P$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -741,7 +787,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Tablas!$I$8:$P$8</c:f>
+              <c:f>'Tablas Mediciones'!$I$8:$P$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2913,7 +2959,7 @@
   <dimension ref="A1:I172"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I173" sqref="I173"/>
     </sheetView>
   </sheetViews>
@@ -2960,16 +3006,16 @@
       <c r="A2" s="10">
         <v>40</v>
       </c>
-      <c r="B2" s="36">
+      <c r="B2" s="34">
         <v>0</v>
       </c>
       <c r="C2" s="10">
         <v>17</v>
       </c>
-      <c r="D2" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="36"/>
+      <c r="D2" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="34"/>
       <c r="F2" s="10">
         <v>67314.5</v>
       </c>
@@ -2981,7 +3027,7 @@
         <f>G2/60</f>
         <v>1.1219083333333333</v>
       </c>
-      <c r="I2" s="36">
+      <c r="I2" s="34">
         <f>SUM(F2:F6)/5</f>
         <v>67096.639999999985</v>
       </c>
@@ -2990,12 +3036,12 @@
       <c r="A3" s="10">
         <v>40</v>
       </c>
-      <c r="B3" s="36"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="10">
         <v>17</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
       <c r="F3" s="10">
         <v>67088.899999999994</v>
       </c>
@@ -3007,18 +3053,18 @@
         <f t="shared" ref="H3:H66" si="1">G3/60</f>
         <v>1.1181483333333333</v>
       </c>
-      <c r="I3" s="36"/>
+      <c r="I3" s="34"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>40</v>
       </c>
-      <c r="B4" s="36"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="10">
         <v>17</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
       <c r="F4" s="10">
         <v>67185.7</v>
       </c>
@@ -3030,18 +3076,18 @@
         <f t="shared" si="1"/>
         <v>1.1197616666666665</v>
       </c>
-      <c r="I4" s="36"/>
+      <c r="I4" s="34"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>40</v>
       </c>
-      <c r="B5" s="36"/>
+      <c r="B5" s="34"/>
       <c r="C5" s="10">
         <v>17</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
       <c r="F5" s="10">
         <v>66607.7</v>
       </c>
@@ -3053,18 +3099,18 @@
         <f t="shared" si="1"/>
         <v>1.1101283333333332</v>
       </c>
-      <c r="I5" s="36"/>
+      <c r="I5" s="34"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>40</v>
       </c>
-      <c r="B6" s="36"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="10">
         <v>17</v>
       </c>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
       <c r="F6" s="10">
         <v>67286.399999999994</v>
       </c>
@@ -3076,7 +3122,7 @@
         <f t="shared" si="1"/>
         <v>1.12144</v>
       </c>
-      <c r="I6" s="36"/>
+      <c r="I6" s="34"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
@@ -3204,16 +3250,16 @@
       <c r="A12" s="6">
         <v>40</v>
       </c>
-      <c r="B12" s="34">
+      <c r="B12" s="36">
         <v>1</v>
       </c>
       <c r="C12" s="6">
         <v>17</v>
       </c>
-      <c r="D12" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="34" t="s">
+      <c r="D12" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="36" t="s">
         <v>17</v>
       </c>
       <c r="F12" s="6">
@@ -3227,7 +3273,7 @@
         <f t="shared" si="1"/>
         <v>1.1233633333333335</v>
       </c>
-      <c r="I12" s="34">
+      <c r="I12" s="36">
         <f t="shared" ref="I12" si="2">SUM(F12:F16)/5</f>
         <v>66700.5</v>
       </c>
@@ -3236,12 +3282,12 @@
       <c r="A13" s="6">
         <v>40</v>
       </c>
-      <c r="B13" s="34"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="6">
         <v>17</v>
       </c>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
       <c r="F13" s="6">
         <v>66515</v>
       </c>
@@ -3253,18 +3299,18 @@
         <f t="shared" si="1"/>
         <v>1.1085833333333333</v>
       </c>
-      <c r="I13" s="34"/>
+      <c r="I13" s="36"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>40</v>
       </c>
-      <c r="B14" s="34"/>
+      <c r="B14" s="36"/>
       <c r="C14" s="6">
         <v>17</v>
       </c>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
       <c r="F14" s="6">
         <v>66720.3</v>
       </c>
@@ -3276,18 +3322,18 @@
         <f t="shared" si="1"/>
         <v>1.1120050000000001</v>
       </c>
-      <c r="I14" s="34"/>
+      <c r="I14" s="36"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>40</v>
       </c>
-      <c r="B15" s="34"/>
+      <c r="B15" s="36"/>
       <c r="C15" s="6">
         <v>17</v>
       </c>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
       <c r="F15" s="6">
         <v>66057.2</v>
       </c>
@@ -3299,18 +3345,18 @@
         <f t="shared" si="1"/>
         <v>1.1009533333333332</v>
       </c>
-      <c r="I15" s="34"/>
+      <c r="I15" s="36"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>40</v>
       </c>
-      <c r="B16" s="34"/>
+      <c r="B16" s="36"/>
       <c r="C16" s="6">
         <v>17</v>
       </c>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
       <c r="F16" s="6">
         <v>66808.2</v>
       </c>
@@ -3322,7 +3368,7 @@
         <f t="shared" si="1"/>
         <v>1.11347</v>
       </c>
-      <c r="I16" s="34"/>
+      <c r="I16" s="36"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
@@ -3700,16 +3746,16 @@
       <c r="A32" s="6">
         <v>40</v>
       </c>
-      <c r="B32" s="34">
+      <c r="B32" s="36">
         <v>2</v>
       </c>
       <c r="C32" s="6">
         <v>17</v>
       </c>
-      <c r="D32" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="E32" s="34" t="s">
+      <c r="D32" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="36" t="s">
         <v>17</v>
       </c>
       <c r="F32" s="6">
@@ -3723,7 +3769,7 @@
         <f t="shared" si="1"/>
         <v>0.62847333333333344</v>
       </c>
-      <c r="I32" s="34">
+      <c r="I32" s="36">
         <f t="shared" ref="I32" si="6">SUM(F32:F36)/5</f>
         <v>32993.94</v>
       </c>
@@ -3732,12 +3778,12 @@
       <c r="A33" s="6">
         <v>40</v>
       </c>
-      <c r="B33" s="34"/>
+      <c r="B33" s="36"/>
       <c r="C33" s="6">
         <v>17</v>
       </c>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="36"/>
       <c r="F33" s="6">
         <v>29796.6</v>
       </c>
@@ -3749,18 +3795,18 @@
         <f t="shared" si="1"/>
         <v>0.49660999999999994</v>
       </c>
-      <c r="I33" s="34"/>
+      <c r="I33" s="36"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>40</v>
       </c>
-      <c r="B34" s="34"/>
+      <c r="B34" s="36"/>
       <c r="C34" s="6">
         <v>17</v>
       </c>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="36"/>
       <c r="F34" s="6">
         <v>31599.7</v>
       </c>
@@ -3772,18 +3818,18 @@
         <f t="shared" si="1"/>
         <v>0.52666166666666669</v>
       </c>
-      <c r="I34" s="34"/>
+      <c r="I34" s="36"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>40</v>
       </c>
-      <c r="B35" s="34"/>
+      <c r="B35" s="36"/>
       <c r="C35" s="6">
         <v>17</v>
       </c>
-      <c r="D35" s="34"/>
-      <c r="E35" s="34"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="36"/>
       <c r="F35" s="6">
         <v>28161.8</v>
       </c>
@@ -3795,18 +3841,18 @@
         <f t="shared" si="1"/>
         <v>0.4693633333333333</v>
       </c>
-      <c r="I35" s="34"/>
+      <c r="I35" s="36"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>40</v>
       </c>
-      <c r="B36" s="34"/>
+      <c r="B36" s="36"/>
       <c r="C36" s="6">
         <v>17</v>
       </c>
-      <c r="D36" s="34"/>
-      <c r="E36" s="34"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36"/>
       <c r="F36" s="6">
         <v>37703.199999999997</v>
       </c>
@@ -3818,7 +3864,7 @@
         <f t="shared" si="1"/>
         <v>0.62838666666666654</v>
       </c>
-      <c r="I36" s="34"/>
+      <c r="I36" s="36"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
@@ -4196,16 +4242,16 @@
       <c r="A52" s="6">
         <v>40</v>
       </c>
-      <c r="B52" s="34">
+      <c r="B52" s="36">
         <v>3</v>
       </c>
       <c r="C52" s="6">
         <v>17</v>
       </c>
-      <c r="D52" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="E52" s="34" t="s">
+      <c r="D52" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E52" s="36" t="s">
         <v>17</v>
       </c>
       <c r="F52" s="6">
@@ -4219,7 +4265,7 @@
         <f t="shared" si="1"/>
         <v>0.47929833333333338</v>
       </c>
-      <c r="I52" s="34">
+      <c r="I52" s="36">
         <f t="shared" ref="I52" si="10">SUM(F52:F56)/5</f>
         <v>26377.120000000003</v>
       </c>
@@ -4228,12 +4274,12 @@
       <c r="A53" s="6">
         <v>40</v>
       </c>
-      <c r="B53" s="34"/>
+      <c r="B53" s="36"/>
       <c r="C53" s="6">
         <v>17</v>
       </c>
-      <c r="D53" s="34"/>
-      <c r="E53" s="34"/>
+      <c r="D53" s="36"/>
+      <c r="E53" s="36"/>
       <c r="F53" s="6">
         <v>28475.3</v>
       </c>
@@ -4245,18 +4291,18 @@
         <f t="shared" si="1"/>
         <v>0.47458833333333333</v>
       </c>
-      <c r="I53" s="34"/>
+      <c r="I53" s="36"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="6">
         <v>40</v>
       </c>
-      <c r="B54" s="34"/>
+      <c r="B54" s="36"/>
       <c r="C54" s="6">
         <v>17</v>
       </c>
-      <c r="D54" s="34"/>
-      <c r="E54" s="34"/>
+      <c r="D54" s="36"/>
+      <c r="E54" s="36"/>
       <c r="F54" s="6">
         <v>25300</v>
       </c>
@@ -4268,18 +4314,18 @@
         <f t="shared" si="1"/>
         <v>0.42166666666666669</v>
       </c>
-      <c r="I54" s="34"/>
+      <c r="I54" s="36"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
         <v>40</v>
       </c>
-      <c r="B55" s="34"/>
+      <c r="B55" s="36"/>
       <c r="C55" s="6">
         <v>17</v>
       </c>
-      <c r="D55" s="34"/>
-      <c r="E55" s="34"/>
+      <c r="D55" s="36"/>
+      <c r="E55" s="36"/>
       <c r="F55" s="6">
         <v>20617.3</v>
       </c>
@@ -4291,18 +4337,18 @@
         <f t="shared" si="1"/>
         <v>0.34362166666666666</v>
       </c>
-      <c r="I55" s="34"/>
+      <c r="I55" s="36"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
         <v>40</v>
       </c>
-      <c r="B56" s="34"/>
+      <c r="B56" s="36"/>
       <c r="C56" s="6">
         <v>17</v>
       </c>
-      <c r="D56" s="34"/>
-      <c r="E56" s="34"/>
+      <c r="D56" s="36"/>
+      <c r="E56" s="36"/>
       <c r="F56" s="6">
         <v>28735.1</v>
       </c>
@@ -4314,7 +4360,7 @@
         <f t="shared" si="1"/>
         <v>0.47891833333333333</v>
       </c>
-      <c r="I56" s="34"/>
+      <c r="I56" s="36"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
@@ -4692,16 +4738,16 @@
       <c r="A72" s="6">
         <v>40</v>
       </c>
-      <c r="B72" s="34">
+      <c r="B72" s="36">
         <v>4</v>
       </c>
       <c r="C72" s="6">
         <v>17</v>
       </c>
-      <c r="D72" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="E72" s="34" t="s">
+      <c r="D72" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E72" s="36" t="s">
         <v>17</v>
       </c>
       <c r="F72" s="6">
@@ -4715,7 +4761,7 @@
         <f t="shared" si="14"/>
         <v>0.3953416666666667</v>
       </c>
-      <c r="I72" s="34">
+      <c r="I72" s="36">
         <f t="shared" ref="I72" si="16">SUM(F72:F76)/5</f>
         <v>23896.339999999997</v>
       </c>
@@ -4724,12 +4770,12 @@
       <c r="A73" s="6">
         <v>40</v>
       </c>
-      <c r="B73" s="34"/>
+      <c r="B73" s="36"/>
       <c r="C73" s="6">
         <v>17</v>
       </c>
-      <c r="D73" s="34"/>
-      <c r="E73" s="34"/>
+      <c r="D73" s="36"/>
+      <c r="E73" s="36"/>
       <c r="F73" s="6">
         <v>23819.3</v>
       </c>
@@ -4741,18 +4787,18 @@
         <f t="shared" si="14"/>
         <v>0.39698833333333333</v>
       </c>
-      <c r="I73" s="34"/>
+      <c r="I73" s="36"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="6">
         <v>40</v>
       </c>
-      <c r="B74" s="34"/>
+      <c r="B74" s="36"/>
       <c r="C74" s="6">
         <v>17</v>
       </c>
-      <c r="D74" s="34"/>
-      <c r="E74" s="34"/>
+      <c r="D74" s="36"/>
+      <c r="E74" s="36"/>
       <c r="F74" s="6">
         <v>24014.1</v>
       </c>
@@ -4764,18 +4810,18 @@
         <f t="shared" si="14"/>
         <v>0.40023500000000001</v>
       </c>
-      <c r="I74" s="34"/>
+      <c r="I74" s="36"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="6">
         <v>40</v>
       </c>
-      <c r="B75" s="34"/>
+      <c r="B75" s="36"/>
       <c r="C75" s="6">
         <v>17</v>
       </c>
-      <c r="D75" s="34"/>
-      <c r="E75" s="34"/>
+      <c r="D75" s="36"/>
+      <c r="E75" s="36"/>
       <c r="F75" s="6">
         <v>24041.7</v>
       </c>
@@ -4787,18 +4833,18 @@
         <f t="shared" si="14"/>
         <v>0.40069500000000002</v>
       </c>
-      <c r="I75" s="34"/>
+      <c r="I75" s="36"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="6">
         <v>40</v>
       </c>
-      <c r="B76" s="34"/>
+      <c r="B76" s="36"/>
       <c r="C76" s="6">
         <v>17</v>
       </c>
-      <c r="D76" s="34"/>
-      <c r="E76" s="34"/>
+      <c r="D76" s="36"/>
+      <c r="E76" s="36"/>
       <c r="F76" s="6">
         <v>23886.1</v>
       </c>
@@ -4810,7 +4856,7 @@
         <f t="shared" si="14"/>
         <v>0.39810166666666663</v>
       </c>
-      <c r="I76" s="34"/>
+      <c r="I76" s="36"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="7">
@@ -5188,16 +5234,16 @@
       <c r="A92" s="6">
         <v>40</v>
       </c>
-      <c r="B92" s="34">
+      <c r="B92" s="36">
         <v>5</v>
       </c>
       <c r="C92" s="6">
         <v>17</v>
       </c>
-      <c r="D92" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="E92" s="34" t="s">
+      <c r="D92" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E92" s="36" t="s">
         <v>17</v>
       </c>
       <c r="F92" s="6">
@@ -5211,7 +5257,7 @@
         <f t="shared" si="14"/>
         <v>0.23414499999999999</v>
       </c>
-      <c r="I92" s="34">
+      <c r="I92" s="36">
         <f t="shared" ref="I92" si="20">SUM(F92:F96)/5</f>
         <v>18268.879999999997</v>
       </c>
@@ -5220,12 +5266,12 @@
       <c r="A93" s="6">
         <v>40</v>
       </c>
-      <c r="B93" s="34"/>
+      <c r="B93" s="36"/>
       <c r="C93" s="6">
         <v>17</v>
       </c>
-      <c r="D93" s="34"/>
-      <c r="E93" s="34"/>
+      <c r="D93" s="36"/>
+      <c r="E93" s="36"/>
       <c r="F93" s="6">
         <v>21845.3</v>
       </c>
@@ -5237,18 +5283,18 @@
         <f t="shared" si="14"/>
         <v>0.36408833333333329</v>
       </c>
-      <c r="I93" s="34"/>
+      <c r="I93" s="36"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="6">
         <v>40</v>
       </c>
-      <c r="B94" s="34"/>
+      <c r="B94" s="36"/>
       <c r="C94" s="6">
         <v>17</v>
       </c>
-      <c r="D94" s="34"/>
-      <c r="E94" s="34"/>
+      <c r="D94" s="36"/>
+      <c r="E94" s="36"/>
       <c r="F94" s="6">
         <v>19805.900000000001</v>
       </c>
@@ -5260,18 +5306,18 @@
         <f t="shared" si="14"/>
         <v>0.33009833333333333</v>
       </c>
-      <c r="I94" s="34"/>
+      <c r="I94" s="36"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="6">
         <v>40</v>
       </c>
-      <c r="B95" s="34"/>
+      <c r="B95" s="36"/>
       <c r="C95" s="6">
         <v>17</v>
       </c>
-      <c r="D95" s="34"/>
-      <c r="E95" s="34"/>
+      <c r="D95" s="36"/>
+      <c r="E95" s="36"/>
       <c r="F95" s="6">
         <v>21785.3</v>
       </c>
@@ -5283,18 +5329,18 @@
         <f t="shared" si="14"/>
         <v>0.36308833333333335</v>
       </c>
-      <c r="I95" s="34"/>
+      <c r="I95" s="36"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="6">
         <v>40</v>
       </c>
-      <c r="B96" s="34"/>
+      <c r="B96" s="36"/>
       <c r="C96" s="6">
         <v>17</v>
       </c>
-      <c r="D96" s="34"/>
-      <c r="E96" s="34"/>
+      <c r="D96" s="36"/>
+      <c r="E96" s="36"/>
       <c r="F96" s="6">
         <v>13859.2</v>
       </c>
@@ -5306,7 +5352,7 @@
         <f t="shared" si="14"/>
         <v>0.2309866666666667</v>
       </c>
-      <c r="I96" s="34"/>
+      <c r="I96" s="36"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="7">
@@ -5684,16 +5730,16 @@
       <c r="A112" s="6">
         <v>40</v>
       </c>
-      <c r="B112" s="34">
+      <c r="B112" s="36">
         <v>6</v>
       </c>
       <c r="C112" s="6">
         <v>17</v>
       </c>
-      <c r="D112" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="E112" s="34" t="s">
+      <c r="D112" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E112" s="36" t="s">
         <v>17</v>
       </c>
       <c r="F112" s="6">
@@ -5707,7 +5753,7 @@
         <f t="shared" si="14"/>
         <v>0.34729666666666664</v>
       </c>
-      <c r="I112" s="34">
+      <c r="I112" s="36">
         <f t="shared" ref="I112" si="24">SUM(F112:F116)/5</f>
         <v>20798.82</v>
       </c>
@@ -5716,12 +5762,12 @@
       <c r="A113" s="6">
         <v>40</v>
       </c>
-      <c r="B113" s="34"/>
+      <c r="B113" s="36"/>
       <c r="C113" s="6">
         <v>17</v>
       </c>
-      <c r="D113" s="34"/>
-      <c r="E113" s="34"/>
+      <c r="D113" s="36"/>
+      <c r="E113" s="36"/>
       <c r="F113" s="6">
         <v>20744.900000000001</v>
       </c>
@@ -5733,18 +5779,18 @@
         <f t="shared" si="14"/>
         <v>0.34574833333333338</v>
       </c>
-      <c r="I113" s="34"/>
+      <c r="I113" s="36"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="6">
         <v>40</v>
       </c>
-      <c r="B114" s="34"/>
+      <c r="B114" s="36"/>
       <c r="C114" s="6">
         <v>17</v>
       </c>
-      <c r="D114" s="34"/>
-      <c r="E114" s="34"/>
+      <c r="D114" s="36"/>
+      <c r="E114" s="36"/>
       <c r="F114" s="6">
         <v>20356.099999999999</v>
       </c>
@@ -5756,18 +5802,18 @@
         <f t="shared" si="14"/>
         <v>0.33926833333333328</v>
       </c>
-      <c r="I114" s="34"/>
+      <c r="I114" s="36"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="6">
         <v>40</v>
       </c>
-      <c r="B115" s="34"/>
+      <c r="B115" s="36"/>
       <c r="C115" s="6">
         <v>17</v>
       </c>
-      <c r="D115" s="34"/>
-      <c r="E115" s="34"/>
+      <c r="D115" s="36"/>
+      <c r="E115" s="36"/>
       <c r="F115" s="6">
         <v>20857.900000000001</v>
       </c>
@@ -5779,18 +5825,18 @@
         <f t="shared" si="14"/>
         <v>0.34763166666666667</v>
       </c>
-      <c r="I115" s="34"/>
+      <c r="I115" s="36"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="6">
         <v>40</v>
       </c>
-      <c r="B116" s="34"/>
+      <c r="B116" s="36"/>
       <c r="C116" s="6">
         <v>17</v>
       </c>
-      <c r="D116" s="34"/>
-      <c r="E116" s="34"/>
+      <c r="D116" s="36"/>
+      <c r="E116" s="36"/>
       <c r="F116" s="6">
         <v>21197.4</v>
       </c>
@@ -5802,7 +5848,7 @@
         <f t="shared" si="14"/>
         <v>0.35329000000000005</v>
       </c>
-      <c r="I116" s="34"/>
+      <c r="I116" s="36"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="7">
@@ -6180,16 +6226,16 @@
       <c r="A132" s="6">
         <v>40</v>
       </c>
-      <c r="B132" s="34">
+      <c r="B132" s="36">
         <v>7</v>
       </c>
       <c r="C132" s="6">
         <v>17</v>
       </c>
-      <c r="D132" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="E132" s="34" t="s">
+      <c r="D132" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E132" s="36" t="s">
         <v>17</v>
       </c>
       <c r="F132" s="6">
@@ -6203,7 +6249,7 @@
         <f t="shared" si="29"/>
         <v>0.27372666666666662</v>
       </c>
-      <c r="I132" s="34">
+      <c r="I132" s="36">
         <f t="shared" ref="I132" si="30">SUM(F132:F136)/5</f>
         <v>18812.939999999999</v>
       </c>
@@ -6212,12 +6258,12 @@
       <c r="A133" s="6">
         <v>40</v>
       </c>
-      <c r="B133" s="34"/>
+      <c r="B133" s="36"/>
       <c r="C133" s="6">
         <v>17</v>
       </c>
-      <c r="D133" s="34"/>
-      <c r="E133" s="34"/>
+      <c r="D133" s="36"/>
+      <c r="E133" s="36"/>
       <c r="F133" s="6">
         <v>14398.2</v>
       </c>
@@ -6229,18 +6275,18 @@
         <f t="shared" si="29"/>
         <v>0.23997000000000002</v>
       </c>
-      <c r="I133" s="34"/>
+      <c r="I133" s="36"/>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="6">
         <v>40</v>
       </c>
-      <c r="B134" s="34"/>
+      <c r="B134" s="36"/>
       <c r="C134" s="6">
         <v>17</v>
       </c>
-      <c r="D134" s="34"/>
-      <c r="E134" s="34"/>
+      <c r="D134" s="36"/>
+      <c r="E134" s="36"/>
       <c r="F134" s="6">
         <v>19444.599999999999</v>
       </c>
@@ -6252,18 +6298,18 @@
         <f t="shared" si="29"/>
         <v>0.32407666666666662</v>
       </c>
-      <c r="I134" s="34"/>
+      <c r="I134" s="36"/>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="6">
         <v>40</v>
       </c>
-      <c r="B135" s="34"/>
+      <c r="B135" s="36"/>
       <c r="C135" s="6">
         <v>17</v>
       </c>
-      <c r="D135" s="34"/>
-      <c r="E135" s="34"/>
+      <c r="D135" s="36"/>
+      <c r="E135" s="36"/>
       <c r="F135" s="6">
         <v>21745.8</v>
       </c>
@@ -6275,18 +6321,18 @@
         <f t="shared" si="29"/>
         <v>0.36242999999999997</v>
       </c>
-      <c r="I135" s="34"/>
+      <c r="I135" s="36"/>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="6">
         <v>40</v>
       </c>
-      <c r="B136" s="34"/>
+      <c r="B136" s="36"/>
       <c r="C136" s="6">
         <v>17</v>
       </c>
-      <c r="D136" s="34"/>
-      <c r="E136" s="34"/>
+      <c r="D136" s="36"/>
+      <c r="E136" s="36"/>
       <c r="F136" s="6">
         <v>22052.5</v>
       </c>
@@ -6298,7 +6344,7 @@
         <f t="shared" si="29"/>
         <v>0.36754166666666666</v>
       </c>
-      <c r="I136" s="34"/>
+      <c r="I136" s="36"/>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="7">
@@ -6676,16 +6722,16 @@
       <c r="A152" s="6">
         <v>40</v>
       </c>
-      <c r="B152" s="34">
+      <c r="B152" s="36">
         <v>8</v>
       </c>
       <c r="C152" s="6">
         <v>17</v>
       </c>
-      <c r="D152" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="E152" s="34" t="s">
+      <c r="D152" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E152" s="36" t="s">
         <v>17</v>
       </c>
       <c r="F152" s="6">
@@ -6699,7 +6745,7 @@
         <f t="shared" si="29"/>
         <v>0.34019499999999997</v>
       </c>
-      <c r="I152" s="34">
+      <c r="I152" s="36">
         <f t="shared" ref="I152" si="34">SUM(F152:F156)/5</f>
         <v>18298.580000000002</v>
       </c>
@@ -6708,12 +6754,12 @@
       <c r="A153" s="6">
         <v>40</v>
       </c>
-      <c r="B153" s="34"/>
+      <c r="B153" s="36"/>
       <c r="C153" s="6">
         <v>17</v>
       </c>
-      <c r="D153" s="34"/>
-      <c r="E153" s="34"/>
+      <c r="D153" s="36"/>
+      <c r="E153" s="36"/>
       <c r="F153" s="6">
         <v>19244.900000000001</v>
       </c>
@@ -6725,18 +6771,18 @@
         <f t="shared" si="29"/>
         <v>0.32074833333333336</v>
       </c>
-      <c r="I153" s="34"/>
+      <c r="I153" s="36"/>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" s="6">
         <v>40</v>
       </c>
-      <c r="B154" s="34"/>
+      <c r="B154" s="36"/>
       <c r="C154" s="6">
         <v>17</v>
       </c>
-      <c r="D154" s="34"/>
-      <c r="E154" s="34"/>
+      <c r="D154" s="36"/>
+      <c r="E154" s="36"/>
       <c r="F154" s="6">
         <v>19148.3</v>
       </c>
@@ -6748,18 +6794,18 @@
         <f t="shared" si="29"/>
         <v>0.3191383333333333</v>
       </c>
-      <c r="I154" s="34"/>
+      <c r="I154" s="36"/>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" s="6">
         <v>40</v>
       </c>
-      <c r="B155" s="34"/>
+      <c r="B155" s="36"/>
       <c r="C155" s="6">
         <v>17</v>
       </c>
-      <c r="D155" s="34"/>
-      <c r="E155" s="34"/>
+      <c r="D155" s="36"/>
+      <c r="E155" s="36"/>
       <c r="F155" s="6">
         <v>17883.3</v>
       </c>
@@ -6771,18 +6817,18 @@
         <f t="shared" si="29"/>
         <v>0.29805499999999996</v>
       </c>
-      <c r="I155" s="34"/>
+      <c r="I155" s="36"/>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="6">
         <v>40</v>
       </c>
-      <c r="B156" s="34"/>
+      <c r="B156" s="36"/>
       <c r="C156" s="6">
         <v>17</v>
       </c>
-      <c r="D156" s="34"/>
-      <c r="E156" s="34"/>
+      <c r="D156" s="36"/>
+      <c r="E156" s="36"/>
       <c r="F156" s="6">
         <v>14804.7</v>
       </c>
@@ -6794,7 +6840,7 @@
         <f t="shared" si="29"/>
         <v>0.24674500000000002</v>
       </c>
-      <c r="I156" s="34"/>
+      <c r="I156" s="36"/>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="7">
@@ -7180,119 +7226,6 @@
     </row>
   </sheetData>
   <mergeCells count="136">
-    <mergeCell ref="I57:I61"/>
-    <mergeCell ref="I2:I6"/>
-    <mergeCell ref="I7:I11"/>
-    <mergeCell ref="I12:I16"/>
-    <mergeCell ref="I17:I21"/>
-    <mergeCell ref="I22:I26"/>
-    <mergeCell ref="I27:I31"/>
-    <mergeCell ref="I32:I36"/>
-    <mergeCell ref="I37:I41"/>
-    <mergeCell ref="I42:I46"/>
-    <mergeCell ref="I47:I51"/>
-    <mergeCell ref="I52:I56"/>
-    <mergeCell ref="I117:I121"/>
-    <mergeCell ref="I62:I66"/>
-    <mergeCell ref="I67:I71"/>
-    <mergeCell ref="I72:I76"/>
-    <mergeCell ref="I77:I81"/>
-    <mergeCell ref="I82:I86"/>
-    <mergeCell ref="I87:I91"/>
-    <mergeCell ref="I92:I96"/>
-    <mergeCell ref="I97:I101"/>
-    <mergeCell ref="I102:I106"/>
-    <mergeCell ref="I107:I111"/>
-    <mergeCell ref="I112:I116"/>
-    <mergeCell ref="I152:I156"/>
-    <mergeCell ref="I157:I161"/>
-    <mergeCell ref="I162:I166"/>
-    <mergeCell ref="I167:I171"/>
-    <mergeCell ref="I122:I126"/>
-    <mergeCell ref="I127:I131"/>
-    <mergeCell ref="I132:I136"/>
-    <mergeCell ref="I137:I141"/>
-    <mergeCell ref="I142:I146"/>
-    <mergeCell ref="I147:I151"/>
-    <mergeCell ref="D52:D56"/>
-    <mergeCell ref="D57:D61"/>
-    <mergeCell ref="E57:E61"/>
-    <mergeCell ref="E52:E56"/>
-    <mergeCell ref="D62:D66"/>
-    <mergeCell ref="E62:E66"/>
-    <mergeCell ref="D37:D41"/>
-    <mergeCell ref="E37:E41"/>
-    <mergeCell ref="D42:D46"/>
-    <mergeCell ref="E42:E46"/>
-    <mergeCell ref="D47:D51"/>
-    <mergeCell ref="E47:E51"/>
-    <mergeCell ref="D82:D86"/>
-    <mergeCell ref="E82:E86"/>
-    <mergeCell ref="D87:D91"/>
-    <mergeCell ref="E87:E91"/>
-    <mergeCell ref="D92:D96"/>
-    <mergeCell ref="E92:E96"/>
-    <mergeCell ref="D67:D71"/>
-    <mergeCell ref="E67:E71"/>
-    <mergeCell ref="D72:D76"/>
-    <mergeCell ref="E72:E76"/>
-    <mergeCell ref="D77:D81"/>
-    <mergeCell ref="E77:E81"/>
-    <mergeCell ref="D112:D116"/>
-    <mergeCell ref="E112:E116"/>
-    <mergeCell ref="D117:D121"/>
-    <mergeCell ref="E117:E121"/>
-    <mergeCell ref="D122:D126"/>
-    <mergeCell ref="E122:E126"/>
-    <mergeCell ref="D97:D101"/>
-    <mergeCell ref="E97:E101"/>
-    <mergeCell ref="D102:D106"/>
-    <mergeCell ref="E102:E106"/>
-    <mergeCell ref="D107:D111"/>
-    <mergeCell ref="E107:E111"/>
-    <mergeCell ref="D142:D146"/>
-    <mergeCell ref="E142:E146"/>
-    <mergeCell ref="D147:D151"/>
-    <mergeCell ref="E147:E151"/>
-    <mergeCell ref="D152:D156"/>
-    <mergeCell ref="E152:E156"/>
-    <mergeCell ref="D127:D131"/>
-    <mergeCell ref="E127:E131"/>
-    <mergeCell ref="D132:D136"/>
-    <mergeCell ref="E132:E136"/>
-    <mergeCell ref="D137:D141"/>
-    <mergeCell ref="E137:E141"/>
-    <mergeCell ref="B167:B171"/>
-    <mergeCell ref="B162:B166"/>
-    <mergeCell ref="B157:B161"/>
-    <mergeCell ref="B152:B156"/>
-    <mergeCell ref="B147:B151"/>
-    <mergeCell ref="D157:D161"/>
-    <mergeCell ref="E157:E161"/>
-    <mergeCell ref="D162:D166"/>
-    <mergeCell ref="E162:E166"/>
-    <mergeCell ref="D167:D171"/>
-    <mergeCell ref="E167:E171"/>
-    <mergeCell ref="B117:B121"/>
-    <mergeCell ref="B112:B116"/>
-    <mergeCell ref="B107:B111"/>
-    <mergeCell ref="B102:B106"/>
-    <mergeCell ref="B97:B101"/>
-    <mergeCell ref="B142:B146"/>
-    <mergeCell ref="B137:B141"/>
-    <mergeCell ref="B132:B136"/>
-    <mergeCell ref="B127:B131"/>
-    <mergeCell ref="B122:B126"/>
-    <mergeCell ref="B67:B71"/>
-    <mergeCell ref="B62:B66"/>
-    <mergeCell ref="B57:B61"/>
-    <mergeCell ref="B52:B56"/>
-    <mergeCell ref="B47:B51"/>
-    <mergeCell ref="B92:B96"/>
-    <mergeCell ref="B87:B91"/>
-    <mergeCell ref="B82:B86"/>
-    <mergeCell ref="B77:B81"/>
-    <mergeCell ref="B72:B76"/>
     <mergeCell ref="B17:B21"/>
     <mergeCell ref="B12:B16"/>
     <mergeCell ref="B7:B11"/>
@@ -7316,6 +7249,119 @@
     <mergeCell ref="E12:E16"/>
     <mergeCell ref="D17:D21"/>
     <mergeCell ref="E17:E21"/>
+    <mergeCell ref="B67:B71"/>
+    <mergeCell ref="B62:B66"/>
+    <mergeCell ref="B57:B61"/>
+    <mergeCell ref="B52:B56"/>
+    <mergeCell ref="B47:B51"/>
+    <mergeCell ref="B92:B96"/>
+    <mergeCell ref="B87:B91"/>
+    <mergeCell ref="B82:B86"/>
+    <mergeCell ref="B77:B81"/>
+    <mergeCell ref="B72:B76"/>
+    <mergeCell ref="B117:B121"/>
+    <mergeCell ref="B112:B116"/>
+    <mergeCell ref="B107:B111"/>
+    <mergeCell ref="B102:B106"/>
+    <mergeCell ref="B97:B101"/>
+    <mergeCell ref="B142:B146"/>
+    <mergeCell ref="B137:B141"/>
+    <mergeCell ref="B132:B136"/>
+    <mergeCell ref="B127:B131"/>
+    <mergeCell ref="B122:B126"/>
+    <mergeCell ref="B167:B171"/>
+    <mergeCell ref="B162:B166"/>
+    <mergeCell ref="B157:B161"/>
+    <mergeCell ref="B152:B156"/>
+    <mergeCell ref="B147:B151"/>
+    <mergeCell ref="D157:D161"/>
+    <mergeCell ref="E157:E161"/>
+    <mergeCell ref="D162:D166"/>
+    <mergeCell ref="E162:E166"/>
+    <mergeCell ref="D167:D171"/>
+    <mergeCell ref="E167:E171"/>
+    <mergeCell ref="D142:D146"/>
+    <mergeCell ref="E142:E146"/>
+    <mergeCell ref="D147:D151"/>
+    <mergeCell ref="E147:E151"/>
+    <mergeCell ref="D152:D156"/>
+    <mergeCell ref="E152:E156"/>
+    <mergeCell ref="D127:D131"/>
+    <mergeCell ref="E127:E131"/>
+    <mergeCell ref="D132:D136"/>
+    <mergeCell ref="E132:E136"/>
+    <mergeCell ref="D137:D141"/>
+    <mergeCell ref="E137:E141"/>
+    <mergeCell ref="D112:D116"/>
+    <mergeCell ref="E112:E116"/>
+    <mergeCell ref="D117:D121"/>
+    <mergeCell ref="E117:E121"/>
+    <mergeCell ref="D122:D126"/>
+    <mergeCell ref="E122:E126"/>
+    <mergeCell ref="D97:D101"/>
+    <mergeCell ref="E97:E101"/>
+    <mergeCell ref="D102:D106"/>
+    <mergeCell ref="E102:E106"/>
+    <mergeCell ref="D107:D111"/>
+    <mergeCell ref="E107:E111"/>
+    <mergeCell ref="D82:D86"/>
+    <mergeCell ref="E82:E86"/>
+    <mergeCell ref="D87:D91"/>
+    <mergeCell ref="E87:E91"/>
+    <mergeCell ref="D92:D96"/>
+    <mergeCell ref="E92:E96"/>
+    <mergeCell ref="D67:D71"/>
+    <mergeCell ref="E67:E71"/>
+    <mergeCell ref="D72:D76"/>
+    <mergeCell ref="E72:E76"/>
+    <mergeCell ref="D77:D81"/>
+    <mergeCell ref="E77:E81"/>
+    <mergeCell ref="D52:D56"/>
+    <mergeCell ref="D57:D61"/>
+    <mergeCell ref="E57:E61"/>
+    <mergeCell ref="E52:E56"/>
+    <mergeCell ref="D62:D66"/>
+    <mergeCell ref="E62:E66"/>
+    <mergeCell ref="D37:D41"/>
+    <mergeCell ref="E37:E41"/>
+    <mergeCell ref="D42:D46"/>
+    <mergeCell ref="E42:E46"/>
+    <mergeCell ref="D47:D51"/>
+    <mergeCell ref="E47:E51"/>
+    <mergeCell ref="I152:I156"/>
+    <mergeCell ref="I157:I161"/>
+    <mergeCell ref="I162:I166"/>
+    <mergeCell ref="I167:I171"/>
+    <mergeCell ref="I122:I126"/>
+    <mergeCell ref="I127:I131"/>
+    <mergeCell ref="I132:I136"/>
+    <mergeCell ref="I137:I141"/>
+    <mergeCell ref="I142:I146"/>
+    <mergeCell ref="I147:I151"/>
+    <mergeCell ref="I117:I121"/>
+    <mergeCell ref="I62:I66"/>
+    <mergeCell ref="I67:I71"/>
+    <mergeCell ref="I72:I76"/>
+    <mergeCell ref="I77:I81"/>
+    <mergeCell ref="I82:I86"/>
+    <mergeCell ref="I87:I91"/>
+    <mergeCell ref="I92:I96"/>
+    <mergeCell ref="I97:I101"/>
+    <mergeCell ref="I102:I106"/>
+    <mergeCell ref="I107:I111"/>
+    <mergeCell ref="I112:I116"/>
+    <mergeCell ref="I57:I61"/>
+    <mergeCell ref="I2:I6"/>
+    <mergeCell ref="I7:I11"/>
+    <mergeCell ref="I12:I16"/>
+    <mergeCell ref="I17:I21"/>
+    <mergeCell ref="I22:I26"/>
+    <mergeCell ref="I27:I31"/>
+    <mergeCell ref="I32:I36"/>
+    <mergeCell ref="I37:I41"/>
+    <mergeCell ref="I42:I46"/>
+    <mergeCell ref="I47:I51"/>
+    <mergeCell ref="I52:I56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -7328,8 +7374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7CD5CF8-E0D3-4596-B6F2-746E33A17FA4}">
   <dimension ref="A1:P171"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7355,17 +7401,17 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="36"/>
+      <c r="A2" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="34"/>
       <c r="C2" s="10">
         <v>67314.5</v>
       </c>
-      <c r="D2" s="36">
+      <c r="D2" s="34">
         <v>0</v>
       </c>
-      <c r="E2" s="36">
+      <c r="E2" s="34">
         <f>SUM(C2:C6)/5</f>
         <v>67096.639999999985</v>
       </c>
@@ -7398,13 +7444,13 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="36"/>
-      <c r="B3" s="36"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="10">
         <v>67088.899999999994</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
       <c r="H3" s="32" t="s">
         <v>21</v>
       </c>
@@ -7442,13 +7488,13 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="10">
         <v>67185.7</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
       <c r="H4" s="31" t="s">
         <v>22</v>
       </c>
@@ -7486,13 +7532,13 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="36"/>
-      <c r="B5" s="36"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
       <c r="C5" s="10">
         <v>66607.7</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
       <c r="H5" s="26" t="s">
         <v>23</v>
       </c>
@@ -7530,13 +7576,13 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="36"/>
-      <c r="B6" s="36"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="10">
         <v>67286.399999999994</v>
       </c>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
       <c r="H6" s="27" t="s">
         <v>24</v>
       </c>
@@ -7696,58 +7742,58 @@
       <c r="E11" s="35"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="34" t="s">
+      <c r="A12" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="36" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="6">
         <v>67401.8</v>
       </c>
-      <c r="D12" s="34">
+      <c r="D12" s="36">
         <v>1</v>
       </c>
-      <c r="E12" s="34">
+      <c r="E12" s="36">
         <f>SUM(C12:C16)/5</f>
         <v>66700.5</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="34"/>
-      <c r="B13" s="34"/>
+      <c r="A13" s="36"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="6">
         <v>66515</v>
       </c>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="34"/>
-      <c r="B14" s="34"/>
+      <c r="A14" s="36"/>
+      <c r="B14" s="36"/>
       <c r="C14" s="6">
         <v>66720.3</v>
       </c>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
-      <c r="B15" s="34"/>
+      <c r="A15" s="36"/>
+      <c r="B15" s="36"/>
       <c r="C15" s="6">
         <v>66057.2</v>
       </c>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
-      <c r="B16" s="34"/>
+      <c r="A16" s="36"/>
+      <c r="B16" s="36"/>
       <c r="C16" s="6">
         <v>66808.2</v>
       </c>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
@@ -7912,58 +7958,58 @@
       <c r="E31" s="38"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="B32" s="34" t="s">
+      <c r="A32" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="36" t="s">
         <v>17</v>
       </c>
       <c r="C32" s="6">
         <v>37708.400000000001</v>
       </c>
-      <c r="D32" s="34">
+      <c r="D32" s="36">
         <v>2</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="36">
         <f>SUM(C32:C36)/5</f>
         <v>32993.94</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="34"/>
-      <c r="B33" s="34"/>
+      <c r="A33" s="36"/>
+      <c r="B33" s="36"/>
       <c r="C33" s="6">
         <v>29796.6</v>
       </c>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="36"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="34"/>
-      <c r="B34" s="34"/>
+      <c r="A34" s="36"/>
+      <c r="B34" s="36"/>
       <c r="C34" s="6">
         <v>31599.7</v>
       </c>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="36"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="34"/>
-      <c r="B35" s="34"/>
+      <c r="A35" s="36"/>
+      <c r="B35" s="36"/>
       <c r="C35" s="6">
         <v>28161.8</v>
       </c>
-      <c r="D35" s="34"/>
-      <c r="E35" s="34"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="36"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="34"/>
-      <c r="B36" s="34"/>
+      <c r="A36" s="36"/>
+      <c r="B36" s="36"/>
       <c r="C36" s="6">
         <v>37703.199999999997</v>
       </c>
-      <c r="D36" s="34"/>
-      <c r="E36" s="34"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="33" t="s">
@@ -8128,58 +8174,58 @@
       <c r="E51" s="38"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="B52" s="34" t="s">
+      <c r="A52" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B52" s="36" t="s">
         <v>17</v>
       </c>
       <c r="C52" s="6">
         <v>28757.9</v>
       </c>
-      <c r="D52" s="34">
+      <c r="D52" s="36">
         <v>3</v>
       </c>
-      <c r="E52" s="34">
+      <c r="E52" s="36">
         <f>SUM(C52:C56)/5</f>
         <v>26377.120000000003</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="34"/>
-      <c r="B53" s="34"/>
+      <c r="A53" s="36"/>
+      <c r="B53" s="36"/>
       <c r="C53" s="6">
         <v>28475.3</v>
       </c>
-      <c r="D53" s="34"/>
-      <c r="E53" s="34"/>
+      <c r="D53" s="36"/>
+      <c r="E53" s="36"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="34"/>
-      <c r="B54" s="34"/>
+      <c r="A54" s="36"/>
+      <c r="B54" s="36"/>
       <c r="C54" s="6">
         <v>25300</v>
       </c>
-      <c r="D54" s="34"/>
-      <c r="E54" s="34"/>
+      <c r="D54" s="36"/>
+      <c r="E54" s="36"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="34"/>
-      <c r="B55" s="34"/>
+      <c r="A55" s="36"/>
+      <c r="B55" s="36"/>
       <c r="C55" s="6">
         <v>20617.3</v>
       </c>
-      <c r="D55" s="34"/>
-      <c r="E55" s="34"/>
+      <c r="D55" s="36"/>
+      <c r="E55" s="36"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="34"/>
-      <c r="B56" s="34"/>
+      <c r="A56" s="36"/>
+      <c r="B56" s="36"/>
       <c r="C56" s="6">
         <v>28735.1</v>
       </c>
-      <c r="D56" s="34"/>
-      <c r="E56" s="34"/>
+      <c r="D56" s="36"/>
+      <c r="E56" s="36"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="33" t="s">
@@ -8344,58 +8390,58 @@
       <c r="E71" s="38"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="B72" s="34" t="s">
+      <c r="A72" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B72" s="36" t="s">
         <v>17</v>
       </c>
       <c r="C72" s="6">
         <v>23720.5</v>
       </c>
-      <c r="D72" s="34">
+      <c r="D72" s="36">
         <v>4</v>
       </c>
-      <c r="E72" s="34">
+      <c r="E72" s="36">
         <f>SUM(C72:C76)/5</f>
         <v>23896.339999999997</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="34"/>
-      <c r="B73" s="34"/>
+      <c r="A73" s="36"/>
+      <c r="B73" s="36"/>
       <c r="C73" s="6">
         <v>23819.3</v>
       </c>
-      <c r="D73" s="34"/>
-      <c r="E73" s="34"/>
+      <c r="D73" s="36"/>
+      <c r="E73" s="36"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="34"/>
-      <c r="B74" s="34"/>
+      <c r="A74" s="36"/>
+      <c r="B74" s="36"/>
       <c r="C74" s="6">
         <v>24014.1</v>
       </c>
-      <c r="D74" s="34"/>
-      <c r="E74" s="34"/>
+      <c r="D74" s="36"/>
+      <c r="E74" s="36"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="34"/>
-      <c r="B75" s="34"/>
+      <c r="A75" s="36"/>
+      <c r="B75" s="36"/>
       <c r="C75" s="6">
         <v>24041.7</v>
       </c>
-      <c r="D75" s="34"/>
-      <c r="E75" s="34"/>
+      <c r="D75" s="36"/>
+      <c r="E75" s="36"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="34"/>
-      <c r="B76" s="34"/>
+      <c r="A76" s="36"/>
+      <c r="B76" s="36"/>
       <c r="C76" s="6">
         <v>23886.1</v>
       </c>
-      <c r="D76" s="34"/>
-      <c r="E76" s="34"/>
+      <c r="D76" s="36"/>
+      <c r="E76" s="36"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="33" t="s">
@@ -8560,58 +8606,58 @@
       <c r="E91" s="38"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="B92" s="34" t="s">
+      <c r="A92" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B92" s="36" t="s">
         <v>17</v>
       </c>
       <c r="C92" s="6">
         <v>14048.7</v>
       </c>
-      <c r="D92" s="34">
+      <c r="D92" s="36">
         <v>5</v>
       </c>
-      <c r="E92" s="34">
+      <c r="E92" s="36">
         <f>SUM(C92:C96)/5</f>
         <v>18268.879999999997</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="34"/>
-      <c r="B93" s="34"/>
+      <c r="A93" s="36"/>
+      <c r="B93" s="36"/>
       <c r="C93" s="6">
         <v>21845.3</v>
       </c>
-      <c r="D93" s="34"/>
-      <c r="E93" s="34"/>
+      <c r="D93" s="36"/>
+      <c r="E93" s="36"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="34"/>
-      <c r="B94" s="34"/>
+      <c r="A94" s="36"/>
+      <c r="B94" s="36"/>
       <c r="C94" s="6">
         <v>19805.900000000001</v>
       </c>
-      <c r="D94" s="34"/>
-      <c r="E94" s="34"/>
+      <c r="D94" s="36"/>
+      <c r="E94" s="36"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="34"/>
-      <c r="B95" s="34"/>
+      <c r="A95" s="36"/>
+      <c r="B95" s="36"/>
       <c r="C95" s="6">
         <v>21785.3</v>
       </c>
-      <c r="D95" s="34"/>
-      <c r="E95" s="34"/>
+      <c r="D95" s="36"/>
+      <c r="E95" s="36"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="34"/>
-      <c r="B96" s="34"/>
+      <c r="A96" s="36"/>
+      <c r="B96" s="36"/>
       <c r="C96" s="6">
         <v>13859.2</v>
       </c>
-      <c r="D96" s="34"/>
-      <c r="E96" s="34"/>
+      <c r="D96" s="36"/>
+      <c r="E96" s="36"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="33" t="s">
@@ -8776,58 +8822,58 @@
       <c r="E111" s="38"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="B112" s="34" t="s">
+      <c r="A112" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B112" s="36" t="s">
         <v>17</v>
       </c>
       <c r="C112" s="6">
         <v>20837.8</v>
       </c>
-      <c r="D112" s="34">
+      <c r="D112" s="36">
         <v>6</v>
       </c>
-      <c r="E112" s="34">
+      <c r="E112" s="36">
         <f>SUM(C112:C116)/5</f>
         <v>20798.82</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="34"/>
-      <c r="B113" s="34"/>
+      <c r="A113" s="36"/>
+      <c r="B113" s="36"/>
       <c r="C113" s="6">
         <v>20744.900000000001</v>
       </c>
-      <c r="D113" s="34"/>
-      <c r="E113" s="34"/>
+      <c r="D113" s="36"/>
+      <c r="E113" s="36"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="34"/>
-      <c r="B114" s="34"/>
+      <c r="A114" s="36"/>
+      <c r="B114" s="36"/>
       <c r="C114" s="6">
         <v>20356.099999999999</v>
       </c>
-      <c r="D114" s="34"/>
-      <c r="E114" s="34"/>
+      <c r="D114" s="36"/>
+      <c r="E114" s="36"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" s="34"/>
-      <c r="B115" s="34"/>
+      <c r="A115" s="36"/>
+      <c r="B115" s="36"/>
       <c r="C115" s="6">
         <v>20857.900000000001</v>
       </c>
-      <c r="D115" s="34"/>
-      <c r="E115" s="34"/>
+      <c r="D115" s="36"/>
+      <c r="E115" s="36"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" s="34"/>
-      <c r="B116" s="34"/>
+      <c r="A116" s="36"/>
+      <c r="B116" s="36"/>
       <c r="C116" s="6">
         <v>21197.4</v>
       </c>
-      <c r="D116" s="34"/>
-      <c r="E116" s="34"/>
+      <c r="D116" s="36"/>
+      <c r="E116" s="36"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="33" t="s">
@@ -8992,58 +9038,58 @@
       <c r="E131" s="38"/>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A132" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="B132" s="34" t="s">
+      <c r="A132" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B132" s="36" t="s">
         <v>17</v>
       </c>
       <c r="C132" s="6">
         <v>16423.599999999999</v>
       </c>
-      <c r="D132" s="34">
+      <c r="D132" s="36">
         <v>7</v>
       </c>
-      <c r="E132" s="34">
+      <c r="E132" s="36">
         <f t="shared" ref="E132" si="2">SUM(C132:C136)/5</f>
         <v>18812.939999999999</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A133" s="34"/>
-      <c r="B133" s="34"/>
+      <c r="A133" s="36"/>
+      <c r="B133" s="36"/>
       <c r="C133" s="6">
         <v>14398.2</v>
       </c>
-      <c r="D133" s="34"/>
-      <c r="E133" s="34"/>
+      <c r="D133" s="36"/>
+      <c r="E133" s="36"/>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A134" s="34"/>
-      <c r="B134" s="34"/>
+      <c r="A134" s="36"/>
+      <c r="B134" s="36"/>
       <c r="C134" s="6">
         <v>19444.599999999999</v>
       </c>
-      <c r="D134" s="34"/>
-      <c r="E134" s="34"/>
+      <c r="D134" s="36"/>
+      <c r="E134" s="36"/>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A135" s="34"/>
-      <c r="B135" s="34"/>
+      <c r="A135" s="36"/>
+      <c r="B135" s="36"/>
       <c r="C135" s="6">
         <v>21745.8</v>
       </c>
-      <c r="D135" s="34"/>
-      <c r="E135" s="34"/>
+      <c r="D135" s="36"/>
+      <c r="E135" s="36"/>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A136" s="34"/>
-      <c r="B136" s="34"/>
+      <c r="A136" s="36"/>
+      <c r="B136" s="36"/>
       <c r="C136" s="6">
         <v>22052.5</v>
       </c>
-      <c r="D136" s="34"/>
-      <c r="E136" s="34"/>
+      <c r="D136" s="36"/>
+      <c r="E136" s="36"/>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="33" t="s">
@@ -9208,58 +9254,58 @@
       <c r="E151" s="38"/>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A152" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="B152" s="34" t="s">
+      <c r="A152" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B152" s="36" t="s">
         <v>17</v>
       </c>
       <c r="C152" s="6">
         <v>20411.7</v>
       </c>
-      <c r="D152" s="34">
+      <c r="D152" s="36">
         <v>8</v>
       </c>
-      <c r="E152" s="34">
+      <c r="E152" s="36">
         <f t="shared" ref="E152" si="6">SUM(C152:C156)/5</f>
         <v>18298.580000000002</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A153" s="34"/>
-      <c r="B153" s="34"/>
+      <c r="A153" s="36"/>
+      <c r="B153" s="36"/>
       <c r="C153" s="6">
         <v>19244.900000000001</v>
       </c>
-      <c r="D153" s="34"/>
-      <c r="E153" s="34"/>
+      <c r="D153" s="36"/>
+      <c r="E153" s="36"/>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A154" s="34"/>
-      <c r="B154" s="34"/>
+      <c r="A154" s="36"/>
+      <c r="B154" s="36"/>
       <c r="C154" s="6">
         <v>19148.3</v>
       </c>
-      <c r="D154" s="34"/>
-      <c r="E154" s="34"/>
+      <c r="D154" s="36"/>
+      <c r="E154" s="36"/>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A155" s="34"/>
-      <c r="B155" s="34"/>
+      <c r="A155" s="36"/>
+      <c r="B155" s="36"/>
       <c r="C155" s="6">
         <v>17883.3</v>
       </c>
-      <c r="D155" s="34"/>
-      <c r="E155" s="34"/>
+      <c r="D155" s="36"/>
+      <c r="E155" s="36"/>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A156" s="34"/>
-      <c r="B156" s="34"/>
+      <c r="A156" s="36"/>
+      <c r="B156" s="36"/>
       <c r="C156" s="6">
         <v>14804.7</v>
       </c>
-      <c r="D156" s="34"/>
-      <c r="E156" s="34"/>
+      <c r="D156" s="36"/>
+      <c r="E156" s="36"/>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="33" t="s">
@@ -9425,24 +9471,112 @@
     </row>
   </sheetData>
   <mergeCells count="136">
-    <mergeCell ref="D2:D6"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="D22:D26"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="D27:D31"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="B27:B31"/>
-    <mergeCell ref="D12:D16"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="D17:D21"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="E152:E156"/>
+    <mergeCell ref="E157:E161"/>
+    <mergeCell ref="E162:E166"/>
+    <mergeCell ref="E167:E171"/>
+    <mergeCell ref="E122:E126"/>
+    <mergeCell ref="E127:E131"/>
+    <mergeCell ref="E132:E136"/>
+    <mergeCell ref="E137:E141"/>
+    <mergeCell ref="E142:E146"/>
+    <mergeCell ref="E147:E151"/>
+    <mergeCell ref="E92:E96"/>
+    <mergeCell ref="E97:E101"/>
+    <mergeCell ref="E102:E106"/>
+    <mergeCell ref="E107:E111"/>
+    <mergeCell ref="E112:E116"/>
+    <mergeCell ref="E117:E121"/>
+    <mergeCell ref="E62:E66"/>
+    <mergeCell ref="E67:E71"/>
+    <mergeCell ref="E72:E76"/>
+    <mergeCell ref="E77:E81"/>
+    <mergeCell ref="E82:E86"/>
+    <mergeCell ref="E87:E91"/>
+    <mergeCell ref="E32:E36"/>
+    <mergeCell ref="E37:E41"/>
+    <mergeCell ref="E42:E46"/>
+    <mergeCell ref="E47:E51"/>
+    <mergeCell ref="E52:E56"/>
+    <mergeCell ref="E57:E61"/>
+    <mergeCell ref="E2:E6"/>
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="E12:E16"/>
+    <mergeCell ref="E17:E21"/>
+    <mergeCell ref="E22:E26"/>
+    <mergeCell ref="E27:E31"/>
+    <mergeCell ref="D162:D166"/>
+    <mergeCell ref="A162:A166"/>
+    <mergeCell ref="B162:B166"/>
+    <mergeCell ref="D167:D171"/>
+    <mergeCell ref="A167:A171"/>
+    <mergeCell ref="B167:B171"/>
+    <mergeCell ref="D152:D156"/>
+    <mergeCell ref="A152:A156"/>
+    <mergeCell ref="B152:B156"/>
+    <mergeCell ref="D157:D161"/>
+    <mergeCell ref="A157:A161"/>
+    <mergeCell ref="B157:B161"/>
+    <mergeCell ref="D142:D146"/>
+    <mergeCell ref="A142:A146"/>
+    <mergeCell ref="B142:B146"/>
+    <mergeCell ref="D147:D151"/>
+    <mergeCell ref="A147:A151"/>
+    <mergeCell ref="B147:B151"/>
+    <mergeCell ref="D132:D136"/>
+    <mergeCell ref="A132:A136"/>
+    <mergeCell ref="B132:B136"/>
+    <mergeCell ref="D137:D141"/>
+    <mergeCell ref="A137:A141"/>
+    <mergeCell ref="B137:B141"/>
+    <mergeCell ref="D122:D126"/>
+    <mergeCell ref="A122:A126"/>
+    <mergeCell ref="B122:B126"/>
+    <mergeCell ref="D127:D131"/>
+    <mergeCell ref="A127:A131"/>
+    <mergeCell ref="B127:B131"/>
+    <mergeCell ref="D112:D116"/>
+    <mergeCell ref="A112:A116"/>
+    <mergeCell ref="B112:B116"/>
+    <mergeCell ref="D117:D121"/>
+    <mergeCell ref="A117:A121"/>
+    <mergeCell ref="B117:B121"/>
+    <mergeCell ref="D102:D106"/>
+    <mergeCell ref="A102:A106"/>
+    <mergeCell ref="B102:B106"/>
+    <mergeCell ref="D107:D111"/>
+    <mergeCell ref="A107:A111"/>
+    <mergeCell ref="B107:B111"/>
+    <mergeCell ref="D92:D96"/>
+    <mergeCell ref="A92:A96"/>
+    <mergeCell ref="B92:B96"/>
+    <mergeCell ref="D97:D101"/>
+    <mergeCell ref="A97:A101"/>
+    <mergeCell ref="B97:B101"/>
+    <mergeCell ref="D82:D86"/>
+    <mergeCell ref="A82:A86"/>
+    <mergeCell ref="B82:B86"/>
+    <mergeCell ref="D87:D91"/>
+    <mergeCell ref="A87:A91"/>
+    <mergeCell ref="B87:B91"/>
+    <mergeCell ref="D72:D76"/>
+    <mergeCell ref="A72:A76"/>
+    <mergeCell ref="B72:B76"/>
+    <mergeCell ref="D77:D81"/>
+    <mergeCell ref="A77:A81"/>
+    <mergeCell ref="B77:B81"/>
+    <mergeCell ref="D62:D66"/>
+    <mergeCell ref="A62:A66"/>
+    <mergeCell ref="B62:B66"/>
+    <mergeCell ref="D67:D71"/>
+    <mergeCell ref="A67:A71"/>
+    <mergeCell ref="B67:B71"/>
+    <mergeCell ref="D52:D56"/>
+    <mergeCell ref="A52:A56"/>
+    <mergeCell ref="B52:B56"/>
+    <mergeCell ref="D57:D61"/>
+    <mergeCell ref="A57:A61"/>
+    <mergeCell ref="B57:B61"/>
     <mergeCell ref="D42:D46"/>
     <mergeCell ref="A42:A46"/>
     <mergeCell ref="B42:B46"/>
@@ -9455,112 +9589,24 @@
     <mergeCell ref="D37:D41"/>
     <mergeCell ref="A37:A41"/>
     <mergeCell ref="B37:B41"/>
-    <mergeCell ref="D62:D66"/>
-    <mergeCell ref="A62:A66"/>
-    <mergeCell ref="B62:B66"/>
-    <mergeCell ref="D67:D71"/>
-    <mergeCell ref="A67:A71"/>
-    <mergeCell ref="B67:B71"/>
-    <mergeCell ref="D52:D56"/>
-    <mergeCell ref="A52:A56"/>
-    <mergeCell ref="B52:B56"/>
-    <mergeCell ref="D57:D61"/>
-    <mergeCell ref="A57:A61"/>
-    <mergeCell ref="B57:B61"/>
-    <mergeCell ref="D82:D86"/>
-    <mergeCell ref="A82:A86"/>
-    <mergeCell ref="B82:B86"/>
-    <mergeCell ref="D87:D91"/>
-    <mergeCell ref="A87:A91"/>
-    <mergeCell ref="B87:B91"/>
-    <mergeCell ref="D72:D76"/>
-    <mergeCell ref="A72:A76"/>
-    <mergeCell ref="B72:B76"/>
-    <mergeCell ref="D77:D81"/>
-    <mergeCell ref="A77:A81"/>
-    <mergeCell ref="B77:B81"/>
-    <mergeCell ref="D102:D106"/>
-    <mergeCell ref="A102:A106"/>
-    <mergeCell ref="B102:B106"/>
-    <mergeCell ref="D107:D111"/>
-    <mergeCell ref="A107:A111"/>
-    <mergeCell ref="B107:B111"/>
-    <mergeCell ref="D92:D96"/>
-    <mergeCell ref="A92:A96"/>
-    <mergeCell ref="B92:B96"/>
-    <mergeCell ref="D97:D101"/>
-    <mergeCell ref="A97:A101"/>
-    <mergeCell ref="B97:B101"/>
-    <mergeCell ref="D122:D126"/>
-    <mergeCell ref="A122:A126"/>
-    <mergeCell ref="B122:B126"/>
-    <mergeCell ref="D127:D131"/>
-    <mergeCell ref="A127:A131"/>
-    <mergeCell ref="B127:B131"/>
-    <mergeCell ref="D112:D116"/>
-    <mergeCell ref="A112:A116"/>
-    <mergeCell ref="B112:B116"/>
-    <mergeCell ref="D117:D121"/>
-    <mergeCell ref="A117:A121"/>
-    <mergeCell ref="B117:B121"/>
-    <mergeCell ref="D142:D146"/>
-    <mergeCell ref="A142:A146"/>
-    <mergeCell ref="B142:B146"/>
-    <mergeCell ref="D147:D151"/>
-    <mergeCell ref="A147:A151"/>
-    <mergeCell ref="B147:B151"/>
-    <mergeCell ref="D132:D136"/>
-    <mergeCell ref="A132:A136"/>
-    <mergeCell ref="B132:B136"/>
-    <mergeCell ref="D137:D141"/>
-    <mergeCell ref="A137:A141"/>
-    <mergeCell ref="B137:B141"/>
-    <mergeCell ref="D162:D166"/>
-    <mergeCell ref="A162:A166"/>
-    <mergeCell ref="B162:B166"/>
-    <mergeCell ref="D167:D171"/>
-    <mergeCell ref="A167:A171"/>
-    <mergeCell ref="B167:B171"/>
-    <mergeCell ref="D152:D156"/>
-    <mergeCell ref="A152:A156"/>
-    <mergeCell ref="B152:B156"/>
-    <mergeCell ref="D157:D161"/>
-    <mergeCell ref="A157:A161"/>
-    <mergeCell ref="B157:B161"/>
-    <mergeCell ref="E32:E36"/>
-    <mergeCell ref="E37:E41"/>
-    <mergeCell ref="E42:E46"/>
-    <mergeCell ref="E47:E51"/>
-    <mergeCell ref="E52:E56"/>
-    <mergeCell ref="E57:E61"/>
-    <mergeCell ref="E2:E6"/>
-    <mergeCell ref="E7:E11"/>
-    <mergeCell ref="E12:E16"/>
-    <mergeCell ref="E17:E21"/>
-    <mergeCell ref="E22:E26"/>
-    <mergeCell ref="E27:E31"/>
-    <mergeCell ref="E92:E96"/>
-    <mergeCell ref="E97:E101"/>
-    <mergeCell ref="E102:E106"/>
-    <mergeCell ref="E107:E111"/>
-    <mergeCell ref="E112:E116"/>
-    <mergeCell ref="E117:E121"/>
-    <mergeCell ref="E62:E66"/>
-    <mergeCell ref="E67:E71"/>
-    <mergeCell ref="E72:E76"/>
-    <mergeCell ref="E77:E81"/>
-    <mergeCell ref="E82:E86"/>
-    <mergeCell ref="E87:E91"/>
-    <mergeCell ref="E152:E156"/>
-    <mergeCell ref="E157:E161"/>
-    <mergeCell ref="E162:E166"/>
-    <mergeCell ref="E167:E171"/>
-    <mergeCell ref="E122:E126"/>
-    <mergeCell ref="E127:E131"/>
-    <mergeCell ref="E132:E136"/>
-    <mergeCell ref="E137:E141"/>
-    <mergeCell ref="E142:E146"/>
-    <mergeCell ref="E147:E151"/>
+    <mergeCell ref="D27:D31"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="D12:D16"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="D17:D21"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="D22:D26"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="B22:B26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -9568,4 +9614,1127 @@
   </ignoredErrors>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0788B50F-0C90-4F3F-B45B-288EBFFEEE56}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1CFFCF-4DC2-4551-8A39-F0BEB2AA2EFA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EA062C9-2939-4BA5-98E0-54E86652D22D}">
+  <dimension ref="A1:M101"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:M1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="39" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EDD41A0-C973-4094-85FE-0DEE675700DD}">
+  <dimension ref="A1:G101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="40" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>